<commit_message>
Create data visualizations for power analyses.
</commit_message>
<xml_diff>
--- a/power_analysis_data_2.xlsx
+++ b/power_analysis_data_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Natasha\projects\nest_box_data_collection_study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C18520-2855-4854-8BA5-AE720A1D67CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BE0C89-661D-4FD0-AAAB-A80BDA1084F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5205" yWindow="638" windowWidth="16590" windowHeight="13425" xr2:uid="{EB8B476B-40C5-485A-A7DE-1238BDA315B6}"/>
   </bookViews>
@@ -35,24 +35,6 @@
     <t>sample_size</t>
   </si>
   <si>
-    <t>manova_s</t>
-  </si>
-  <si>
-    <t>manova_m</t>
-  </si>
-  <si>
-    <t>manova_l</t>
-  </si>
-  <si>
-    <t>manova_rpt_s</t>
-  </si>
-  <si>
-    <t>manova_rpt_m</t>
-  </si>
-  <si>
-    <t>manova_rpt_l</t>
-  </si>
-  <si>
     <t>ttest_p_s</t>
   </si>
   <si>
@@ -60,6 +42,24 @@
   </si>
   <si>
     <t>ttest_p_l</t>
+  </si>
+  <si>
+    <t>m3_s</t>
+  </si>
+  <si>
+    <t>m3_m</t>
+  </si>
+  <si>
+    <t>m3_l</t>
+  </si>
+  <si>
+    <t>m_rpt_s</t>
+  </si>
+  <si>
+    <t>m_rpt_m</t>
+  </si>
+  <si>
+    <t>m_rpt_l</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -432,31 +432,31 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">

</xml_diff>